<commit_message>
graficos otras variables en timeseries
</commit_message>
<xml_diff>
--- a/HistRatios.xlsx
+++ b/HistRatios.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="306" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="306" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="pp" sheetId="1" state="visible" r:id="rId2"/>
@@ -245,12 +245,12 @@
   </sheetPr>
   <dimension ref="A1:AA58"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="N40" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="E41" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
-      <selection pane="bottomRight" activeCell="S59" activeCellId="0" sqref="S59"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+      <selection pane="bottomRight" activeCell="B45" activeCellId="1" sqref="W43:W58 B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4026,10 +4026,10 @@
       </c>
       <c r="V45" s="3" t="n">
         <f aca="false">(dw!V45*100)/dw!S45</f>
-        <v>13.2798383518683</v>
+        <v>12.2773977166939</v>
       </c>
       <c r="W45" s="3" t="n">
-        <v>0.839104948168606</v>
+        <v>0.339104948168606</v>
       </c>
       <c r="X45" s="3" t="n">
         <v>0.398673461425525</v>
@@ -5154,12 +5154,12 @@
   </sheetPr>
   <dimension ref="A1:AA58"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="4" ySplit="1" topLeftCell="N38" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T54" activeCellId="0" sqref="T54"/>
+      <selection pane="bottomLeft" activeCell="A38" activeCellId="0" sqref="A38"/>
+      <selection pane="bottomRight" activeCell="W43" activeCellId="0" sqref="W43:W58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -8920,7 +8920,7 @@
         <v>0.268100569298955</v>
       </c>
       <c r="C45" s="3" t="n">
-        <v>0.0514072227645998</v>
+        <v>0.4214072227646</v>
       </c>
       <c r="D45" s="3" t="n">
         <v>0.965141669560864</v>
@@ -8969,7 +8969,7 @@
       </c>
       <c r="S45" s="3" t="n">
         <f aca="false">SUM(B45:R45)</f>
-        <v>4.53157722839748</v>
+        <v>4.90157722839748</v>
       </c>
       <c r="T45" s="3" t="n">
         <v>1.37820225694989</v>
@@ -8982,7 +8982,7 @@
         <v>0.601786130721259</v>
       </c>
       <c r="W45" s="3" t="n">
-        <v>0.839104948168606</v>
+        <v>0.388828918809728</v>
       </c>
       <c r="X45" s="3" t="n">
         <v>0.398673461425525</v>
@@ -9407,7 +9407,7 @@
         <v>2.80288001568757</v>
       </c>
       <c r="W50" s="3" t="n">
-        <v>0.77294712797797</v>
+        <v>0.37294712797797</v>
       </c>
       <c r="X50" s="3" t="n">
         <v>0.088965374788931</v>

</xml_diff>

<commit_message>
corregi algoritmo calculo de reactivities
</commit_message>
<xml_diff>
--- a/HistRatios.xlsx
+++ b/HistRatios.xlsx
@@ -271,7 +271,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R1" activeCellId="0" sqref="R1"/>
+      <selection pane="bottomRight" activeCell="R1" activeCellId="1" sqref="S16:V16 R1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5119,7 +5119,7 @@
   <dimension ref="A1:AA58"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D11" activeCellId="1" sqref="S16:V16 D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9960,7 +9960,7 @@
   <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="topLeft" activeCell="I14" activeCellId="1" sqref="S16:V16 I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -10266,8 +10266,8 @@
   </sheetPr>
   <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D18" activeCellId="0" sqref="D18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="J1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="S16" activeCellId="0" sqref="S16:V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -10538,7 +10538,7 @@
         <v>67.8617998142836</v>
       </c>
       <c r="T4" s="0" t="n">
-        <v>10.9129196010073</v>
+        <v>10.5295949146195</v>
       </c>
       <c r="U4" s="0" t="n">
         <v>8.0191581486404</v>
@@ -11082,7 +11082,7 @@
         <v>6.87160650947841</v>
       </c>
       <c r="T12" s="0" t="n">
-        <v>64.8390199587196</v>
+        <v>64.581336793845</v>
       </c>
       <c r="U12" s="0" t="n">
         <v>7.05133247144246</v>
@@ -11150,7 +11150,7 @@
         <v>5.12425965848062</v>
       </c>
       <c r="T13" s="0" t="n">
-        <v>64.4323380367871</v>
+        <v>64.2859219942657</v>
       </c>
       <c r="U13" s="0" t="n">
         <v>4.97697969327783</v>
@@ -11218,7 +11218,7 @@
         <v>7.66209246300504</v>
       </c>
       <c r="T14" s="0" t="n">
-        <v>62.6977160021973</v>
+        <v>62.4765339683172</v>
       </c>
       <c r="U14" s="0" t="n">
         <v>6.56826763159372</v>
@@ -11286,7 +11286,7 @@
         <v>9.49456722803815</v>
       </c>
       <c r="T15" s="0" t="n">
-        <v>65.733021033708</v>
+        <v>65.4856873762657</v>
       </c>
       <c r="U15" s="0" t="n">
         <v>6.61628466486838</v>
@@ -11354,13 +11354,13 @@
         <v>7.02142654590977</v>
       </c>
       <c r="T16" s="0" t="n">
-        <v>63.4463240176412</v>
+        <v>63.315302402957</v>
       </c>
       <c r="U16" s="0" t="n">
         <v>10.2976429745875</v>
       </c>
       <c r="V16" s="0" t="n">
-        <v>19.3656280765458</v>
+        <v>19.3656280765457</v>
       </c>
     </row>
   </sheetData>

</xml_diff>